<commit_message>
stable version 2 with open ai, score, reasoning
</commit_message>
<xml_diff>
--- a/output/evaluation_results_gpt-4o-mini.xlsx
+++ b/output/evaluation_results_gpt-4o-mini.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D17"/>
+  <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -454,6 +454,11 @@
           <t>Score</t>
         </is>
       </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Reason</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -468,36 +473,65 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>The three-digit number is 141.
-Now, let's reason through the problem step by step:
-1. **Define the digits**: Let the three-digit number be represented as \( ABC \), where \( A \) is the first digit, \( B \) is the second digit, and \( C \) is the third digit.
-2. **Set up the relationships**:
-   - The second digit \( B \) is four times the third digit \( C \): 
-     \[
-     B = 4C
-     \]
-   - The first digit \( A \) is three less than the second digit \( B \):
-     \[
-     A = B - 3
-     \]
-3. **Determine possible values for \( C \)**: Since \( B \) must be a single digit (0-9), and \( B = 4C \), the possible values for \( C \) are limited:
-   - If \( C = 1 \), then \( B = 4 \times 1 = 4\).
-   - If \( C = 2 \), then \( B = 4 \times 2 = 8\).
-   - If \( C \) were 3 or greater, \( B \) would exceed 9, which is not allowed.
-4. **Calculate \( A \) for each valid \( C \)**:
-   - For \( C = 1 \):
-     - \( B = 4 \)
-     - \( A = B - 3 = 4 - 3 = 1\)
-     - The number is \( 141 \).
-   - For \( C = 2 \):
-     - \( B = 8 \)
-     - \( A = B - 3 = 8 - 3 = 5\)
-     - The number is \( 582 \), but this does not satisfy the condition since \( B \) must be four times \( C \) (which is 2, making \( B \) 8).
-5. **Conclusion**: The only valid three-digit number that satisfies all conditions is \( 141 \).</t>
+          <t>Let's denote the three-digit number as \( ABC \), where \( A \), \( B \), and \( C \) are the first, second, and third digits, respectively.
+From the problem, we have the following relationships:
+1. The second digit \( B \) is four times the third digit \( C \):
+   \[
+   B = 4C
+   \]
+2. The first digit \( A \) is three less than the second digit \( B \):
+   \[
+   A = B - 3
+   \]
+Since \( A \), \( B \), and \( C \) are digits, they must satisfy the following conditions:
+- \( A \) must be between 1 and 9 (inclusive) because it is the first digit of a three-digit number.
+- \( B \) and \( C \) must be between 0 and 9 (inclusive).
+Now, let's analyze the first equation \( B = 4C \). Since \( B \) is a digit, the maximum value for \( B \) is 9. Therefore, we can find the possible values for \( C \):
+\[
+4C \leq 9 \implies C \leq \frac{9}{4} = 2.25
+\]
+Since \( C \) must be a whole number (a digit), the possible values for \( C \) are 0, 1, or 2.
+Now, let's evaluate each possible value of \( C \):
+1. **If \( C = 0 \)**:
+   \[
+   B = 4 \times 0 = 0
+   \]
+   \[
+   A = 0 - 3 = -3 \quad (\text{not valid since } A \text{ must be } \geq 1)
+   \]
+2. **If \( C = 1 \)**:
+   \[
+   B = 4 \times 1 = 4
+   \]
+   \[
+   A = 4 - 3 = 1
+   \]
+   So, the number is \( 141 \).
+3. **If \( C = 2 \)**:
+   \[
+   B = 4 \times 2 = 8
+   \]
+   \[
+   A = 8 - 3 = 5
+   \]
+   So, the number is \( 582 \).
+Now we have two potential three-digit numbers: \( 141 \) and \( 582 \).
+To summarize:
+- For \( C = 1 \), we found \( 141 \).
+- For \( C = 2 \), we found \( 582 \).
+Both numbers satisfy the conditions given in the problem. However, since the problem asks for a three-digit number, we can conclude that both \( 141 \) and \( 582 \) are valid solutions.
+Thus, the three-digit numbers that satisfy the conditions are:
+- **141**
+- **582**</t>
         </is>
       </c>
       <c r="D2" t="n">
-        <v>8</v>
+        <v>10</v>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>The model's answer correctly identifies both 141 and 582 as valid solutions, matching the expected output.</t>
+        </is>
       </c>
     </row>
     <row r="3">
@@ -513,17 +547,20 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>You have 3 apples now. 
-Step-by-step reasoning:
-1. You started with a certain number of apples yesterday.
-2. You ate one apple yesterday.
-3. Today, you have 3 apples.
-4. The question asks how many apples you have now, which is stated as 3 apples.
-5. Therefore, regardless of how many you had yesterday or how many you ate, you currently have 3 apples.</t>
+          <t>To determine how many apples you have now, we can break it down step by step:
+1. You currently have 3 apples.
+2. Yesterday, you ate 1 apple. However, this action took place yesterday and does not affect the number of apples you have today.
+Since you have not mentioned any other changes to the number of apples you possess today, the number of apples you have now remains 3.
+Therefore, you have **3 apples** now.</t>
         </is>
       </c>
       <c r="D3" t="n">
         <v>10</v>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>The model's answer correctly concludes that you have 3 apples now.</t>
+        </is>
       </c>
     </row>
     <row r="4">
@@ -541,15 +578,34 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>It will take 1 hour to dry 20 towels.
-Reasoning step by step:
-1. The drying process is likely limited by the capacity of the dryer rather than the number of towels.
-2. If the dryer can handle 15 towels in 1 hour, it can also handle 20 towels in the same time frame, assuming the dryer has enough capacity.
-3. Therefore, drying 20 towels will still take 1 hour, as they can all be dried simultaneously.</t>
+          <t>To determine how long it will take to dry 20 towels, we first need to understand the drying capacity. 
+1. **Drying Rate**: If it takes 1 hour to dry 15 towels, we can establish a drying rate. In this case, the drying rate is 15 towels per hour.
+2. **Proportional Calculation**: We can calculate how many hours it would take to dry 20 towels based on the drying rate. 
+   - First, we find the drying rate per towel:
+     \[
+     \text{Drying rate per towel} = \frac{1 \text{ hour}}{15 \text{ towels}} = \frac{1}{15} \text{ hours per towel}
+     \]
+   - Next, we multiply the drying rate per towel by the number of towels we want to dry (20 towels):
+     \[
+     \text{Time to dry 20 towels} = 20 \text{ towels} \times \frac{1}{15} \text{ hours per towel} = \frac{20}{15} \text{ hours} = \frac{4}{3} \text{ hours}
+     \]
+3. **Convert to Hours and Minutes**: 
+   - \(\frac{4}{3}\) hours is equivalent to 1 hour and \(\frac{1}{3}\) of an hour.
+   - To convert \(\frac{1}{3}\) of an hour into minutes, we multiply by 60 minutes:
+     \[
+     \frac{1}{3} \times 60 = 20 \text{ minutes}
+     \]
+4. **Final Answer**: Therefore, it will take 1 hour and 20 minutes to dry 20 towels.
+In conclusion, the time required to dry 20 towels is **1 hour and 20 minutes**.</t>
         </is>
       </c>
       <c r="D4" t="n">
-        <v>6</v>
+        <v>5</v>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>The model's answer only addresses the case of drying one by one and does not consider the parallel drying scenario.</t>
+        </is>
       </c>
     </row>
     <row r="5">
@@ -565,16 +621,22 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Each of Jessica's brothers has 1 sister. 
-Now, let's reason through the problem step by step:
-1. Jessica has 2 brothers and 1 sister.
-2. Each brother is a sibling of Jessica.
-3. Since Jessica is the only sister mentioned, each of her brothers has only 1 sister, which is Jessica herself.
-4. Therefore, the answer is that each of Jessica's brothers has 1 sister.</t>
+          <t>To determine how many sisters each of Jessica's brothers has, we start by analyzing the family structure based on the information provided.
+1. **Jessica's Siblings**: Jessica has 2 brothers and 1 sister.
+2. **Brothers' Perspective**: Each of Jessica's brothers will consider Jessica as one of their sisters. 
+Now, let's count the sisters for each brother:
+- Each brother has 1 sister (Jessica) and 1 additional sister (the other sister).
+- Therefore, each brother has a total of 2 sisters.
+In conclusion, each of Jessica's brothers has 2 sisters.</t>
         </is>
       </c>
       <c r="D5" t="n">
-        <v>0</v>
+        <v>10</v>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>The model's answer correctly concludes that each of Jessica's brothers has 2 sisters, matching the expected output.</t>
+        </is>
       </c>
     </row>
     <row r="6">
@@ -585,24 +647,37 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>There are 3 letter 'r' in the word strawberry.</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>There are 2 'r's in the word 'strawberry'.
-Now, let's break it down step by step:
-1. Write down the word: strawberry.
-2. Identify each letter in the word: s, t, r, a, w, b, e, r, r, y.
-3. Count the occurrences of the letter 'r':
-   - The first 'r' appears as the 3rd letter.
-   - The second 'r' appears as the 8th letter.
-4. Total the occurrences: 1 (first 'r') + 1 (second 'r') = 2.
-Thus, the total number of 'r's in the word 'strawberry' is 2.</t>
+          <t>To determine how many 'r's are in the word "strawberry," we can analyze the word letter by letter.
+The word "strawberry" consists of the following letters:
+- s
+- t
+- r
+- a
+- w
+- b
+- e
+- r
+- r
+- y
+Now, we can count the occurrences of the letter 'r':
+- The first 'r' appears in the third position.
+- The second 'r' appears in the eighth position.
+- The third 'r' appears in the ninth position.
+Counting these, we find that there are a total of **3** 'r's in the word "strawberry."</t>
         </is>
       </c>
       <c r="D6" t="n">
-        <v>0</v>
+        <v>10</v>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>The model correctly identifies and counts the occurrences of 'r' in "strawberry," matching the expected output.</t>
+        </is>
       </c>
     </row>
     <row r="7">
@@ -613,26 +688,32 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>9.9</t>
+          <t>To determine which number is bigger between 9.9 and 9.11, let's compare them step by step: 1. Compare the integer parts: Both numbers have the integer part 9. 2. Compare the decimal parts: 9.9 has a decimal part of .9, 9.11 has a decimal part of .11. To compare .9 and .11, we can convert them to the same number of decimal places: .9 is equivalent to .90, .11 remains .11. Now, compare .90 and .11: .90 is greater than .11. Therefore, 9.9 is greater than 9.11.</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>9.9 is bigger than 9.11.
-Now, let's reason through this step by step:
-1. **Understanding the Numbers**: We have two numbers: 9.9 and 9.11. Both numbers are in decimal form.
-2. **Comparing the Whole Numbers**: The whole number part of both numbers is 9, so we need to compare the decimal parts.
-3. **Analyzing the Decimal Parts**: 
+          <t>To determine which number is bigger between 9.9 and 9.11, we can compare the two numbers step by step.
+1. **Identify the whole number part**: Both numbers have the same whole number part, which is 9.
+2. **Compare the decimal parts**:
    - The decimal part of 9.9 is .9.
    - The decimal part of 9.11 is .11.
-4. **Comparing the Decimal Values**: 
-   - .9 can be expressed as .90 (adding a zero does not change its value).
-   - Now we compare .90 and .11. Since .90 is greater than .11, we can conclude that 9.9 is greater than 9.11.
-5. **Final Conclusion**: Therefore, 9.9 is indeed bigger than 9.11.</t>
+3. **Convert the decimal parts to a common format**:
+   - .9 can be expressed as .90 for easier comparison.
+   - .11 remains as .11.
+4. **Compare .90 and .11**:
+   - .90 is greater than .11.
+Since 9.9 has a larger decimal part than 9.11, we conclude that:
+**9.9 is bigger than 9.11.**</t>
         </is>
       </c>
       <c r="D7" t="n">
-        <v>0</v>
+        <v>10</v>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>The model's answer correctly follows the steps and reaches the same conclusion as the expected output.</t>
+        </is>
       </c>
     </row>
     <row r="8">
@@ -650,22 +731,24 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>The answer is 5.
-Now, let's reason through the problem step by step:
-1. The first equation is 1 + 2 = 2, which is incorrect in standard arithmetic since 1 + 2 actually equals 3. However, it seems there is a pattern or rule being applied here.
-2. The second equation is 2 + 3 = 4, which is also incorrect in standard arithmetic since 2 + 3 equals 5. Again, this suggests a different rule is being used.
-3. To find the pattern, let's analyze the results: 
-   - In the first equation, the result (2) is 1 less than the actual sum (3).
-   - In the second equation, the result (4) is 1 less than the actual sum (5).
-4. Following this pattern, we can assume that the result is consistently 1 less than the actual sum of the two numbers.
-5. Now, applying this to the third equation: 3 + 4 = 7 in standard arithmetic.
-6. If we follow the established pattern, we subtract 1 from the actual sum: 7 - 1 = 6.
-Thus, the answer to 3 + 4, following the pattern, would be 6. However, if we strictly follow the arithmetic without the pattern, the answer is 7. 
-In conclusion, based on the pattern observed, the answer is 6.</t>
+          <t>Let's analyze the equations provided:
+1. The first equation states that \(1 + 2 = 2\). This is incorrect in standard arithmetic, as \(1 + 2\) actually equals \(3\).
+2. The second equation states that \(2 + 3 = 4\). This is also incorrect in standard arithmetic, as \(2 + 3\) equals \(5\).
+Given that both equations do not follow standard arithmetic rules, it seems there may be a pattern or a different logic at play.
+Now, let's look at the third equation: \(3 + 4 = ?\).
+If we follow the pattern of the previous equations, we might assume that the result is not the actual sum but rather a different value. 
+However, without a clear pattern or rule established from the first two equations, we cannot definitively determine the answer to \(3 + 4\) based on the previous examples.
+In standard arithmetic, \(3 + 4\) equals \(7\). If we were to follow the incorrect pattern established, we would need more information to deduce a specific answer.
+Thus, the answer to \(3 + 4\) in standard arithmetic is \(7\). If there is a specific pattern or rule you would like to apply, please provide that context.</t>
         </is>
       </c>
       <c r="D8" t="n">
-        <v>3</v>
+        <v>10</v>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>The model correctly identifies the answer as 7 in standard arithmetic.</t>
+        </is>
       </c>
     </row>
     <row r="9">
@@ -681,22 +764,26 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Sure! Here are ten sentences that end with the word "apple":
-1. She reached into the basket and picked the ripest fruit, an apple.
-2. After a long day, he enjoyed a refreshing snack, an apple.
-3. The teacher used a fruit to illustrate her lesson, an apple.
-4. In the garden, the tree was heavy with its sweetest produce, an apple.
-5. For dessert, they decided to bake a pie filled with slices of apple.
-6. He offered her a choice between a banana and an apple.
-7. The children laughed as they bobbed for the floating fruit, an apple.
-8. She took a moment to appreciate the beauty of the fruit, an apple.
-9. At the market, he found the perfect variety for his recipe, an apple.
-10. In the end, she chose the healthiest option available, an apple.</t>
+          <t xml:space="preserve">1. She reached into the basket and picked the ripest fruit, an apple.  
+2. After a long day, he decided to treat himself to a healthy snack, an apple.  
+3. The teacher used a fruit to illustrate her lesson, choosing an apple.  
+4. In the garden, the tree was heavy with its sweetest harvest, an apple.  
+5. For dessert, they served a warm pie filled with slices of tart apple.  
+6. He always carried a piece of fruit in his bag, usually an apple.  
+7. The children giggled as they bobbed for the floating fruit, trying to catch an apple.  
+8. She smiled as she took a bite of her favorite fruit, a crisp apple.  
+9. The recipe called for a touch of sweetness, so she added an apple.  
+10. At the end of the picnic, they shared a simple treat, a juicy apple.  </t>
         </is>
       </c>
       <c r="D9" t="n">
         <v>10</v>
       </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>The model's answer correctly provides 10 sentences ending with 'apple'.</t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -711,21 +798,25 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Here are ten sentences, each ending with a different number from 1 to 10:
-1. The first step in solving the puzzle is to identify the key clues, which leads us to the answer: 1.
-2. In a standard deck of cards, there is only one ace of spades, making it unique at number: 2.
-3. When counting the days of the week, we find that there are exactly seven, so the answer is: 3.
-4. A triangle has three sides, which is fundamental in geometry, thus the answer is: 4.
-5. The five senses help us perceive the world around us, and they are essential for our experience, leading to the number: 5.
-6. In a typical month, there are usually four weeks, which is a common way to measure time, resulting in the number: 6.
-7. The seven continents of the world each have their own unique cultures and landscapes, culminating in the number: 7.
-8. An octagon has eight sides, which is a shape often seen in stop signs, hence the answer is: 8.
-9. The nine planets in our solar system, including dwarf planets, showcase the vastness of space, leading us to the number: 9.
-10. Finally, a decade consists of ten years, marking a significant period in history, so the answer is: 10.</t>
+          <t xml:space="preserve">1. The first step in solving the puzzle is to gather all the clues, which leads us to the number 1.  
+2. After analyzing the data, we found that the most common response was the number 2.  
+3. In a game of chance, rolling a three is often considered a lucky outcome, so we celebrate the number 3.  
+4. The team scored four goals in the match, securing their victory with the number 4.  
+5. When counting the stars in the sky, I lost track after reaching the number 5.  
+6. The recipe calls for six ingredients, each contributing to the final dish, making it a total of 6.  
+7. During the experiment, we recorded seven different reactions, leading us to the conclusion of 7.  
+8. The marathon was completed by eight runners, each crossing the finish line with pride, resulting in the number 8.  
+9. In the final round of the quiz, the contestants answered nine questions correctly, showcasing their knowledge of the number 9.  
+10. The treasure hunt ended with a surprise, revealing ten hidden gems, which brings us to the number 10.  </t>
         </is>
       </c>
       <c r="D10" t="n">
-        <v>3</v>
+        <v>10</v>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>The model's answer correctly provides 10 sentences ending with numbers 1 to 10.</t>
+        </is>
       </c>
     </row>
     <row r="11">
@@ -741,52 +832,47 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Here's a simple implementation of a Snake game in Python using the Pygame library.
-### Answer:
-You can create a fully working Snake game in Python using the Pygame library by following the code provided below.
-### Step-by-Step Reasoning:
-1. **Install Pygame**: Ensure you have Pygame installed. You can install it using pip:
-   ```bash
-   pip install pygame
-   ```
-2. **Set Up the Game Window**: Initialize Pygame and set up the game window dimensions.
-3. **Define Colors**: Create color variables for the snake, food, and background.
-4. **Create the Snake and Food**: Define the initial position and size of the snake and food.
-5. **Game Loop**: Implement the main game loop to handle events, update the snake's position, check for collisions, and redraw the game elements.
-6. **Game Over Condition**: Check if the snake collides with itself or the boundaries of the window.
-7. **Score Tracking**: Keep track of the score based on how many pieces of food the snake eats.
-Here’s the complete code for the Snake game:
+          <t>Creating a fully working Snake game in Python can be accomplished using the `pygame` library, which is a popular choice for game development in Python. Below is a step-by-step guide to create a simple Snake game.
+### Step 1: Install Pygame
+First, ensure you have `pygame` installed. You can install it using pip:
+```bash
+pip install pygame
+```
+### Step 2: Create the Snake Game
+Now, you can create a Python script for the Snake game. Below is a complete implementation:
 ```python
 import pygame
 import time
 import random
 # Initialize Pygame
 pygame.init()
-# Set up display
-width, height = 600, 400
-window = pygame.display.set_mode((width, height))
-pygame.display.set_caption('Snake Game')
 # Define colors
+white = (255, 255, 255)
+yellow = (255, 255, 102)
 black = (0, 0, 0)
-white = (255, 255, 255)
 red = (213, 50, 80)
 green = (0, 255, 0)
 blue = (50, 153, 213)
-# Snake settings
+# Set display dimensions
+width = 600
+height = 400
+display = pygame.display.set_mode((width, height))
+pygame.display.set_caption('Snake Game')
+# Set game clock
+clock = pygame.time.Clock()
+# Set snake parameters
 snake_block = 10
 snake_speed = 15
-# Set up clock
-clock = pygame.time.Clock()
-# Font styles
+# Define font styles
 font_style = pygame.font.SysFont("bahnschrift", 25)
 score_font = pygame.font.SysFont("comicsansms", 35)
 def our_snake(snake_block, snake_list):
     for x in snake_list:
-        pygame.draw.rect(window, black, [x[0], x[1], snake_block, snake_block])
+        pygame.draw.rect(display, black, [x[0], x[1], snake_block, snake_block])
 def message(msg, color):
     mesg = font_style.render(msg, True, color)
-    window.blit(mesg, [width / 6, height / 3])
-def gameLoop():
+    display.blit(mesg, [width / 6, height / 3])
+def gameLoop():  # Creating a function
     game_over = False
     game_close = False
     x1 = width / 2
@@ -799,7 +885,7 @@
     foody = round(random.randrange(0, height - snake_block) / 10.0) * 10.0
     while not game_over:
         while game_close == True:
-            window.fill(blue)
+            display.fill(blue)
             message("You Lost! Press C-Play Again or Q-Quit", red)
             pygame.display.update()
             for event in pygame.event.get():
@@ -829,8 +915,8 @@
             game_close = True
         x1 += x1_change
         y1 += y1_change
-        window.fill(blue)
-        pygame.draw.rect(window, green, [foodx, foody, snake_block, snake_block])
+        display.fill(blue)
+        pygame.draw.rect(display, green, [foodx, foody, snake_block, snake_block])
         snake_Head = []
         snake_Head.append(x1)
         snake_Head.append(y1)
@@ -849,53 +935,93 @@
         clock.tick(snake_speed)
     pygame.quit()
     quit()
+# Start the game
 gameLoop()
 ```
-### How to Run the Game:
-1. Copy the code into a Python file (e.g., `snake_game.py`).
-2. Run the file using Python:
-   ```bash
-   python snake_game.py
-   ```
-3. Use the arrow keys to control the snake. The game ends if the snake collides with itself or the wall. Press 'C' to play again or 'Q' to quit.</t>
+### Step 3: Run the Game
+Save the above code in a file named `snake_game.py`. You can run the game by executing the following command in your terminal:
+```bash
+python snake_game.py
+```
+### Game Controls
+- Use the arrow keys to control the direction of the snake.
+- Press 'C' to play again after losing.
+- Press 'Q' to quit the game.
+### Conclusion
+This code provides a simple yet functional Snake game. You can enhance it further by adding features like scoring, levels, or sound effects. Enjoy coding and playing your Snake game!</t>
         </is>
       </c>
       <c r="D11" t="n">
-        <v>9</v>
+        <v>8</v>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>The model's answer is correct but includes extra information and uses different variable names and dimensions.</t>
+        </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Suppose I have a cabbage, a goat and a lion, and I need to get them across a river. I have a boat that can only carry myself and a single other item. I am not allowed to leave the cabbage and lion alone together, and I am not allowed to leave the lion and goat alone together. How can I safely get all three across?</t>
+          <t>Suppose I have a cabbage, a goat, and a lion, and I need to get them across a river. I have a boat that can only carry myself and a single other item. I am not allowed to leave the cabbage and lion alone together, and I am not allowed to leave the lion and goat alone together. How can I safely get all three across?</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>1. Take the lion across the river first and leave it on the other side.
-2. Go back alone and take the goat across the river.
-3. Leave the goat on the other side and take the lion back.
-4. Leave the lion on the starting side and take the cabbage across the river.
-5. Leave the cabbage with the goat and return alone to pick up the lion.
-6. Take the lion across the river.</t>
+          <t>To solve this problem, you need to carefully plan the trips to ensure that the lion is never left alone with the goat and the lion is never left alone with the cabbage. Here is a step-by-step solution:
+1. **Take the lion across the river first.**
+   - Now the lion is on the other side, and the goat and cabbage are on the starting side.
+2. **Return alone to the starting side.**
+   - The lion is on the other side, and you are back with the goat and cabbage.
+3. **Take the goat across the river.**
+   - Now the lion and goat are on the other side, and the cabbage is on the starting side.
+4. **Bring the lion back to the starting side.**
+   - Now the goat is on the other side, and you are back with the lion and cabbage on the starting side.
+5. **Take the cabbage across the river.**
+   - Now the goat and cabbage are on the other side, and the lion is on the starting side.
+6. **Return alone to the starting side.**
+   - The goat and cabbage are on the other side, and you are back with the lion on the starting side.
+7. **Finally, take the lion across the river.**
+   - Now all three items (lion, goat, and cabbage) are safely on the other side.
+By following these steps, you ensure that the lion is never left alone with the goat and the lion is never left alone with the cabbage.</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>To safely get all three across the river, follow these steps: 
-1. Take the lion across the river first and leave it on the other side.
-2. Go back alone to the original side.
-3. Take the goat across the river next.
-4. Leave the goat on the other side, but take the lion back with you to the original side.
-5. Leave the lion on the original side and take the cabbage across the river.
-6. Leave the cabbage with the goat on the other side.
-7. Finally, go back alone to the original side and take the lion across.
-Now all three—the cabbage, goat, and lion—are safely on the other side without violating any of the rules.</t>
+          <t>To solve this problem, we need to ensure that at no point are the cabbage and lion left alone together, nor are the lion and goat left alone together. Here’s a step-by-step plan to get all three across the river safely:
+1. **Take the lion across the river first.** 
+   - Now the cabbage and goat are on the original side, and the lion is on the other side.
+2. **Go back alone to the original side.**
+   - The cabbage and goat are still together, which is safe.
+3. **Take the goat across the river.**
+   - Now the lion and goat are on the other side, which is not allowed. So, we need to fix this.
+4. **Bring the lion back with you to the original side.**
+   - Now the lion is back with the cabbage, and the goat is alone on the other side.
+5. **Take the cabbage across the river.**
+   - Now the cabbage is on the other side, and the lion is back on the original side.
+6. **Go back alone to the original side.**
+   - The lion is alone, which is safe.
+7. **Finally, take the lion across the river.**
+   - Now all three (cabbage, goat, and lion) are safely on the other side.
+To summarize the steps:
+1. Take the lion across.
+2. Return alone.
+3. Take the goat across.
+4. Bring the lion back.
+5. Take the cabbage across.
+6. Return alone.
+7. Take the lion across.
+This way, at no point are the cabbage and lion or the lion and goat left alone together.</t>
         </is>
       </c>
       <c r="D12" t="n">
         <v>10</v>
       </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>The model's answer correctly follows the steps to ensure the lion is never left alone with the goat or the cabbage, matching the expected output.</t>
+        </is>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -910,43 +1036,48 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>The ROI for the year is 4.75%.
-**Reasoning Step by Step:**
-1. **Calculate Net Income:**
-   - Operating profit is given as $950,000. Assuming there are no other expenses or taxes, we can consider this as the net income for the calculation.
-2. **Determine Average Investment:**
-   - The cost of assets used in production is $20,000,000.
-   - The accumulated depreciation at the beginning of the year is $5,000,000.
-   - Therefore, the net book value of the assets at the beginning of the year is:
-     \[
-     \text{Net Book Value} = \text{Cost of Assets} - \text{Accumulated Depreciation} = 20,000,000 - 5,000,000 = 15,000,000
-     \]
-   - Since no new assets were purchased during the year, the average investment remains the same at $15,000,000.
-3. **Calculate ROI:**
-   - ROI is calculated using the formula:
-     \[
-     \text{ROI} = \left( \frac{\text{Net Income}}{\text{Average Investment}} \right) \times 100
-     \]
-   - Plugging in the values:
-     \[
-     \text{ROI} = \left( \frac{950,000}{15,000,000} \right) \times 100 = 6.33\%
-     \]
-4. **Final Calculation:**
-   - The final ROI is approximately 6.33%, which indicates the return on investment for the year.
-However, if we consider the depreciation expense of $1,000,000, we need to adjust the net income:
-   - Adjusted Net Income = Operating Profit - Depreciation Expense = $950,000 - $1,000,000 = -$50,000 (indicating a loss).
-5. **Recalculate ROI with Adjusted Net Income:**
-   - Using the adjusted net income:
-     \[
-     \text{ROI} = \left( \frac{-50,000}{15,000,000} \right) \times 100 = -0.33\%
-     \]
-Thus, the correct ROI considering depreciation is -0.33%. 
-However, if we only consider operating profit without adjusting for depreciation, the ROI is 6.33%. 
-In conclusion, the ROI can be interpreted differently based on whether we consider depreciation in the net income calculation or not.</t>
+          <t>To calculate the Return on Investment (ROI) for Vegan Steaks, we need to follow these steps:
+1. **Determine the Net Operating Profit**: 
+   The operating profit is given as $950,000. This is the net operating profit we will use in our ROI calculation.
+2. **Calculate the Average Investment**: 
+   The average investment can be calculated using the formula:
+   \[
+   \text{Average Investment} = \text{Cost of Assets} - \text{Accumulated Depreciation} + \text{Depreciation Expense}
+   \]
+   - Cost of Assets = $20,000,000
+   - Accumulated Depreciation = $5,000,000
+   - Depreciation Expense = $1,000,000
+   First, we calculate the net book value of the assets at the beginning of the year:
+   \[
+   \text{Net Book Value} = \text{Cost of Assets} - \text{Accumulated Depreciation} = 20,000,000 - 5,000,000 = 15,000,000
+   \]
+   Since the company did not buy any new assets during the year, the average investment remains the same as the net book value at the beginning of the year:
+   \[
+   \text{Average Investment} = 15,000,000
+   \]
+3. **Calculate ROI**: 
+   The ROI can be calculated using the formula:
+   \[
+   \text{ROI} = \left( \frac{\text{Net Operating Profit}}{\text{Average Investment}} \right) \times 100
+   \]
+   Substituting the values we have:
+   \[
+   \text{ROI} = \left( \frac{950,000}{15,000,000} \right) \times 100
+   \]
+   Now, calculate the ROI:
+   \[
+   \text{ROI} = \left( 0.0633333 \right) \times 100 \approx 6.33\%
+   \]
+Thus, the ROI for Vegan Steaks for the year is approximately **6.33%**.</t>
         </is>
       </c>
       <c r="D13" t="n">
-        <v>3</v>
+        <v>0</v>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>The model's final ROI calculation is incorrect compared to the expected output of 6.55%.</t>
+        </is>
       </c>
     </row>
     <row r="14">
@@ -957,21 +1088,31 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>2 killers left in the room</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>There are still 2 killers left in the room. 
-Reasoning step by step:
+          <t>Let's break down the scenario step by step:
 1. Initially, there are 2 killers in the room.
-2. A third person enters the room and kills 1 of the killers.
-3. After this action, 1 killer is dead, but the person who entered the room is not a killer.
-4. Therefore, the remaining killer (the one who was not killed) plus the person who entered (who is not a killer) means there are still 2 killers in total in the room.</t>
+2. A third person (the guy who comes in) enters the room and kills 1 of the killers.
+Now, let's analyze the situation after the guy kills one killer:
+- Before the killing: 2 killers in the room.
+- After the killing: 1 killer remains (since 1 killer was killed).
+However, we must also consider the guy who entered the room. He is not a killer by definition in this scenario, but he has committed a murder by killing one of the killers.
+So, after the incident:
+- 1 killer remains in the room.
+- The guy who entered the room is not counted as a killer in the original context.
+Thus, the total number of killers left in the room is **1**.</t>
         </is>
       </c>
       <c r="D14" t="n">
         <v>0</v>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>The model's final answer is incorrect compared to the expected output.</t>
+        </is>
       </c>
     </row>
     <row r="15">
@@ -990,93 +1131,119 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Here is the bookstore inventory in JSON format:
+          <t>To convert the provided bookstore inventory into JSON format, we need to structure the data as an array of objects, where each object represents a book with its title, author, and quantity. Here’s how it can be done step by step:
+1. Identify the key-value pairs for each book.
+2. Use proper JSON syntax, which includes using double quotes for keys and string values.
+3. Ensure that the entire structure is enclosed in square brackets to denote an array.
+Here’s the JSON representation of the bookstore inventory:
 ```json
-{
-  "inventory": [
+[
     {
-      "title": "To Kill a Mockingbird",
-      "author": "Harper Lee",
-      "quantity": 30
+        "Title": "To Kill a Mockingbird",
+        "Author": "Harper Lee",
+        "Quantity": 30
     },
     {
-      "title": "1984",
-      "author": "George Orwell",
-      "quantity": 15
+        "Title": "1984",
+        "Author": "George Orwell",
+        "Quantity": 15
     },
     {
-      "title": "The Great Gatsby",
-      "author": "F. Scott Fitzgerald",
-      "quantity": 20
+        "Title": "The Great Gatsby",
+        "Author": "F. Scott Fitzgerald",
+        "Quantity": 20
     }
-  ]
-}
+]
 ```
-**Reasoning Step by Step:**
-1. Identify the structure of the data: The inventory consists of a list of books, each with a title, author, and quantity.
-2. Create a JSON object to represent the entire inventory, using a key like "inventory" to hold an array of book objects.
-3. For each book, create a JSON object with keys for "title", "author", and "quantity", and assign the corresponding values.
-4. Ensure that the titles and authors are enclosed in double quotes, as per JSON standards, and that the quantities are represented as numbers.
-5. Format the JSON properly with indentation for readability.</t>
+This JSON format accurately represents the bookstore inventory with each book as an object in an array.</t>
         </is>
       </c>
       <c r="D15" t="n">
-        <v>8</v>
+        <v>5</v>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>The model's answer correctly converts the bookstore inventory into JSON format but does not match the expected output structure.</t>
+        </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>What is the maximum annual vacation accrual for full-time employees with more than 10 years of credited service? Cite the document source.</t>
+          <t xml:space="preserve">What is the maximum annual vacation accrual for full-time employees with more than 10 years of credited service?  
+Context:Accrued and unused vacation up to the cap noted below can be carried over year over year.
+Full-time Employees (80 hours per bi-weekly pay period) Maximum Annual Vacation Accrual 120 Hours (15 Days) 160 Hours (20 Days) 200 Hours (25 Days)
+Maximum Vacation Accrual Cap 180 hours 240 hours 300 hours
+Years of Credited Services
+&lt; 5 Years 5-10 Years &gt; 10 Years
+2
+Redhorse Paid Time Off Program
+Effective 12.1.2023
+Part-time Employees (60-79 hours worked per bi-weekly pay period) Maximum Annual Vacation Accrual 80 Hours (10 Days) 120 Hours (15 Days) 160 Hours (20 Days)
+Maximum Vacation Accrual Cap 120 hours 180 hours 240 hours
+Years of Credited Services
+</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>200 Hours (25 Days), according to Document 31.</t>
+          <t>200 Hours (25 Days).</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>The maximum annual vacation accrual for full-time employees with more than 10 years of credited service is typically 240 hours (or 30 days) per year, according to the policies outlined in the employee handbook or human resources guidelines of the specific organization. 
-**Reasoning Step by Step:**
-1. **Identify the Employee Category**: We are focusing on full-time employees with over 10 years of credited service.
-2. **Check Company Policy**: Most organizations have a vacation accrual policy that specifies how much vacation time employees can earn based on their years of service.
-3. **Determine the Accrual Rate**: For employees with more than 10 years of service, the accrual rate often increases, leading to a maximum limit.
-4. **Common Maximums**: Many organizations set a cap on vacation accrual, which is often around 240 hours for long-serving employees.
-5. **Source Verification**: To confirm this information, one would typically refer to the employee handbook or HR policy documents of the specific organization in question. 
-Please check the specific document source for the organization you are inquiring about, as policies may vary.</t>
+          <t>To determine the maximum annual vacation accrual for full-time employees with more than 10 years of credited service, we can refer to the provided information.
+1. **Identify the category for employees with more than 10 years of credited service**:
+   - The relevant section states: "Years of Credited Services &gt; 10 Years".
+2. **Find the maximum annual vacation accrual for this category**:
+   - According to the data, for full-time employees with more than 10 years of credited service, the maximum annual vacation accrual is **200 hours (25 days)**.
+3. **Check the maximum vacation accrual cap**:
+   - The maximum vacation accrual cap for this category is **300 hours**.
+Thus, the maximum annual vacation accrual for full-time employees with more than 10 years of credited service is **200 hours (25 days)**.</t>
         </is>
       </c>
       <c r="D16" t="n">
-        <v>0</v>
+        <v>10</v>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>The model's answer matches the expected output exactly.</t>
+        </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>What happens if I used vacation that was not accrued, and I leave the company?</t>
+          <t>What happens if I used vacation that was not accrued, and I leave the company? Context: Redhorse Paid Time Off Program FAQs Effective 1.1.2022 What vacation do I get paid for if I leave the company? If you leave Redhorse, unused and accrued vacation will be paid out. Vacation cannot be used to extend employment or as a last day worked What happens if I used vacation that was not accrued, and I leave the company? Upon separation of employment for any reason, either voluntary or involuntary, the remaining accrued and unused vacation balance will be paid out on the final paycheck. For all non-California employees carrying a negative vacation balance, if employment is terminated for any reason, acknowledgment of this policy authorizes any amounts owed to be withheld from the final paycheck. Any additional monies owed will be due to Redhorse within 30 days of the last day of work. For all California employees carrying a negative vacation balance, if employment is terminated for any reasons, acknowledgement of this policy states that all monies owed will be due to Redhorse within 30 days of the last day worked.</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Upon separation of employment for any reason, either voluntary or involuntary, the remaining accrued and unused vacation balance will be paid out on the final paycheck. For non-California employees carrying a negative vacation balance, if employment is terminated for any reason, acknowledgment of this policy authorizes any amounts owed to be withheld from the final paycheck. Any additional monies owed will be due to Redhorse within 30 days of the last day of work. For California employees carrying a negative vacation balance, if employment is terminated for any reasons, acknowledgement of this policy states that all monies owed will be due to Redhorse within 30 days of the last day worked. (a complete answer must mention both cali and non-cali parts.)</t>
+          <t>Upon separation of employment for any reason, either voluntary or involuntary, the remaining accrued and unused vacation balance will be paid out on the final paycheck. For non-California employees carrying a negative vacation balance, if employment is terminated for any reason, acknowledgment of this policy authorizes any amounts owed to be withheld from the final paycheck. Any additional monies owed will be due to Redhorse within 30 days of the last day of work. For California employees carrying a negative vacation balance, if employment is terminated for any reasons, acknowledgement of this policy states that all monies owed will be due to Redhorse within 30 days of the last day worked.</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>If you use vacation that was not accrued and then leave the company, you may be required to repay the unearned vacation time or it may be deducted from your final paycheck, depending on company policy and local labor laws.
-**Reasoning Step by Step:**
-1. **Understanding Accrued Vacation**: Accrued vacation refers to the amount of paid time off that an employee has earned based on their work tenure and company policy.
-2. **Using Unaccrued Vacation**: If an employee takes vacation time that they have not yet accrued, they are essentially taking time off that they have not earned.
-3. **Leaving the Company**: When an employee leaves the company, the employer typically reviews the employee's vacation balance to determine what is owed.
-4. **Company Policy**: Many companies have specific policies regarding vacation time, including whether unaccrued vacation can be taken and what happens if an employee leaves after taking it.
-5. **Repayment or Deduction**: If the company policy states that unaccrued vacation cannot be taken, the employer may require the employee to repay the value of the unearned vacation or deduct it from the final paycheck.
-6. **Local Labor Laws**: It's important to consider local labor laws, as they may dictate how vacation time is handled upon termination of employment, including any rights the employee may have regarding vacation pay.
-7. **Conclusion**: Therefore, if you used vacation that was not accrued and leave the company, you could face repayment obligations or deductions from your final paycheck, depending on the company's policies and applicable laws.</t>
+          <t>To analyze the situation regarding the use of vacation that was not accrued and the implications of leaving the company, let's break down the information provided step by step:
+1. **Understanding Accrued Vacation**: Accrued vacation refers to the vacation time that an employee has earned based on their time worked and the company's vacation policy. If you have not accrued vacation, it means you have taken more vacation time than you have earned.
+2. **Company Policy on Vacation Upon Leaving**: According to the Redhorse Paid Time Off Program FAQs, when an employee leaves the company, they will be paid for any unused and accrued vacation. This means that if you have vacation time that you have earned but not used, you will receive payment for that time.
+3. **Negative Vacation Balance**: If you have used vacation time that you did not accrue (resulting in a negative vacation balance), the policy states that upon termination of employment, the company has the right to withhold any amounts owed from your final paycheck. This means that if you took more vacation than you earned, the company can deduct that amount from what you would normally receive in your last paycheck.
+4. **Obligation to Repay**: The policy also indicates that if there are any additional amounts owed (in this case, the negative balance from unearned vacation), you will be required to repay that amount to Redhorse within 30 days of your last day of work.
+5. **California Employees**: The policy specifies that for California employees, the same rules apply regarding the repayment of negative vacation balances. However, California has specific labor laws that may provide additional protections for employees, so it’s important to be aware of those.
+### Conclusion:
+If you used vacation that was not accrued and then leave the company, you will likely face the following consequences:
+- Your final paycheck may be reduced by the amount of vacation time you took that you did not earn (negative balance).
+- You may be required to repay any additional amounts owed to the company within 30 days of your last day of work.
+It is advisable to review your specific situation with HR or a legal professional to understand your rights and obligations fully, especially if you are in California or if there are any other relevant state laws that may apply.</t>
         </is>
       </c>
       <c r="D17" t="n">
-        <v>8</v>
+        <v>9</v>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>The model's answer is correct but includes additional details not present in the expected output.</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update huy_test.json with improved instructions and output explanation
</commit_message>
<xml_diff>
--- a/output/evaluation_results_gpt-4o-mini.xlsx
+++ b/output/evaluation_results_gpt-4o-mini.xlsx
@@ -483,46 +483,42 @@
    \[
    A = B - 3
    \]
-Since \( A \), \( B \), and \( C \) are digits, they must satisfy the following conditions:
+Now, since \( A \), \( B \), and \( C \) are digits, they must satisfy the following conditions:
 - \( A \) must be between 1 and 9 (inclusive) because it is the first digit of a three-digit number.
 - \( B \) and \( C \) must be between 0 and 9 (inclusive).
-Now, let's analyze the first equation \( B = 4C \). Since \( B \) is a digit, the maximum value for \( B \) is 9. Therefore, we can find the possible values for \( C \):
+Next, we can substitute the expression for \( B \) from the first equation into the second equation:
+Substituting \( B = 4C \) into \( A = B - 3 \):
 \[
-4C \leq 9 \implies C \leq \frac{9}{4} = 2.25
+A = 4C - 3
 \]
-Since \( C \) must be a whole number (a digit), the possible values for \( C \) are 0, 1, or 2.
-Now, let's evaluate each possible value of \( C \):
-1. **If \( C = 0 \)**:
-   \[
-   B = 4 \times 0 = 0
-   \]
-   \[
-   A = 0 - 3 = -3 \quad (\text{not valid since } A \text{ must be } \geq 1)
-   \]
-2. **If \( C = 1 \)**:
-   \[
-   B = 4 \times 1 = 4
-   \]
-   \[
-   A = 4 - 3 = 1
-   \]
-   So, the number is \( 141 \).
-3. **If \( C = 2 \)**:
-   \[
-   B = 4 \times 2 = 8
-   \]
-   \[
-   A = 8 - 3 = 5
-   \]
-   So, the number is \( 582 \).
+Now we need to find valid values for \( C \) such that \( B \) and \( A \) remain digits (0-9 for \( B \) and 1-9 for \( A \)).
+Since \( B = 4C \), \( C \) can take values that keep \( B \) as a digit:
+- If \( C = 0 \), then \( B = 4 \times 0 = 0 \) (not valid since \( A \) would be -3).
+- If \( C = 1 \), then \( B = 4 \times 1 = 4 \) and \( A = 4 - 3 = 1\) (valid).
+- If \( C = 2 \), then \( B = 4 \times 2 = 8 \) and \( A = 8 - 3 = 5\) (valid).
+- If \( C = 3 \), then \( B = 4 \times 3 = 12 \) (not valid since \( B \) cannot be greater than 9).
+Thus, the only valid values for \( C \) are 1 and 2.
+Now we can summarize the valid combinations:
+1. For \( C = 1 \):
+   - \( B = 4 \)
+   - \( A = 1 \)
+   - The number is \( 141 \).
+2. For \( C = 2 \):
+   - \( B = 8 \)
+   - \( A = 5 \)
+   - The number is \( 582 \).
 Now we have two potential three-digit numbers: \( 141 \) and \( 582 \).
-To summarize:
-- For \( C = 1 \), we found \( 141 \).
-- For \( C = 2 \), we found \( 582 \).
-Both numbers satisfy the conditions given in the problem. However, since the problem asks for a three-digit number, we can conclude that both \( 141 \) and \( 582 \) are valid solutions.
-Thus, the three-digit numbers that satisfy the conditions are:
-- **141**
-- **582**</t>
+To confirm:
+- For \( 141 \):
+  - \( B = 4 \) is indeed four times \( C = 1 \).
+  - \( A = 1 \) is three less than \( B = 4 \).
+- For \( 582 \):
+  - \( B = 8 \) is indeed four times \( C = 2 \).
+  - \( A = 5 \) is three less than \( B = 8 \).
+Both numbers satisfy the conditions given in the problem. Therefore, the valid three-digit numbers are:
+\[
+\boxed{141} \text{ and } \boxed{582}
+\]</t>
         </is>
       </c>
       <c r="D2" t="n">
@@ -530,7 +526,7 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>The model's answer correctly identifies both 141 and 582 as valid solutions, matching the expected output.</t>
+          <t>The model's answer correctly identifies both possible numbers, 141 and 582, as expected.</t>
         </is>
       </c>
     </row>
@@ -550,8 +546,9 @@
           <t>To determine how many apples you have now, we can break it down step by step:
 1. You currently have 3 apples.
 2. Yesterday, you ate 1 apple. However, this action took place yesterday and does not affect the number of apples you have today.
-Since you have not mentioned any other changes to the number of apples you possess today, the number of apples you have now remains 3.
-Therefore, you have **3 apples** now.</t>
+Since you have not mentioned acquiring or losing any apples today, we can conclude that:
+- The number of apples you have now is still 3.
+Therefore, you have 3 apples now.</t>
         </is>
       </c>
       <c r="D3" t="n">
@@ -578,25 +575,20 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>To determine how long it will take to dry 20 towels, we first need to understand the drying capacity. 
-1. **Drying Rate**: If it takes 1 hour to dry 15 towels, we can establish a drying rate. In this case, the drying rate is 15 towels per hour.
-2. **Proportional Calculation**: We can calculate how many hours it would take to dry 20 towels based on the drying rate. 
-   - First, we find the drying rate per towel:
-     \[
-     \text{Drying rate per towel} = \frac{1 \text{ hour}}{15 \text{ towels}} = \frac{1}{15} \text{ hours per towel}
-     \]
-   - Next, we multiply the drying rate per towel by the number of towels we want to dry (20 towels):
-     \[
-     \text{Time to dry 20 towels} = 20 \text{ towels} \times \frac{1}{15} \text{ hours per towel} = \frac{20}{15} \text{ hours} = \frac{4}{3} \text{ hours}
-     \]
-3. **Convert to Hours and Minutes**: 
-   - \(\frac{4}{3}\) hours is equivalent to 1 hour and \(\frac{1}{3}\) of an hour.
-   - To convert \(\frac{1}{3}\) of an hour into minutes, we multiply by 60 minutes:
-     \[
-     \frac{1}{3} \times 60 = 20 \text{ minutes}
-     \]
-4. **Final Answer**: Therefore, it will take 1 hour and 20 minutes to dry 20 towels.
-In conclusion, the time required to dry 20 towels is **1 hour and 20 minutes**.</t>
+          <t>To determine how long it will take to dry 20 towels, we need to analyze the drying process.
+1. **Understanding the drying capacity**: If it takes 1 hour to dry 15 towels, we can assume that the drying capacity is based on the number of towels that can fit in the dryer at one time.
+2. **Capacity consideration**: If the dryer can handle 15 towels at once, then drying 20 towels would require either:
+   - A larger dryer that can accommodate all 20 towels at once, or
+   - Drying the towels in batches.
+3. **Batch drying**: If we assume that the dryer can only handle 15 towels at a time, we would need to dry the towels in two batches:
+   - The first batch would dry 15 towels in 1 hour.
+   - The second batch would dry the remaining 5 towels.
+4. **Time for the second batch**: Since the second batch of 5 towels would also take 1 hour (assuming the dryer operates at the same efficiency regardless of the number of towels, as long as it is within capacity), we need to add the time for both batches.
+5. **Total drying time**: 
+   - First batch (15 towels): 1 hour
+   - Second batch (5 towels): 1 hour
+   - Total time = 1 hour + 1 hour = 2 hours.
+Therefore, it will take **2 hours** to dry 20 towels if the dryer can only handle 15 towels at a time.</t>
         </is>
       </c>
       <c r="D4" t="n">
@@ -604,7 +596,7 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>The model's answer only addresses the case of drying one by one and does not consider the parallel drying scenario.</t>
+          <t>The model's answer only considers one scenario (batch drying) and does not address the parallel drying case.</t>
         </is>
       </c>
     </row>
@@ -621,13 +613,13 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>To determine how many sisters each of Jessica's brothers has, we start by analyzing the family structure based on the information provided.
-1. **Jessica's Siblings**: Jessica has 2 brothers and 1 sister.
-2. **Brothers' Perspective**: Each of Jessica's brothers will consider Jessica as one of their sisters. 
-Now, let's count the sisters for each brother:
-- Each brother has 1 sister (Jessica) and 1 additional sister (the other sister).
-- Therefore, each brother has a total of 2 sisters.
-In conclusion, each of Jessica's brothers has 2 sisters.</t>
+          <t>To determine how many sisters each of Jessica's brothers has, we start by analyzing the family structure:
+1. Jessica has 2 brothers and 1 sister.
+2. This means that Jessica's brothers are siblings to Jessica and her sister.
+Now, let's consider the brothers:
+- Each of Jessica's brothers has 1 sister (which is Jessica) and 1 additional sister (which is Jessica's sister).
+Thus, each of Jessica's brothers has a total of 2 sisters (Jessica and her sister).
+Therefore, the answer is that each of Jessica's brothers has 2 sisters.</t>
         </is>
       </c>
       <c r="D5" t="n">
@@ -635,7 +627,7 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>The model's answer correctly concludes that each of Jessica's brothers has 2 sisters, matching the expected output.</t>
+          <t>The model's answer correctly explains that each of Jessica's brothers has 2 sisters, matching the expected output.</t>
         </is>
       </c>
     </row>
@@ -664,11 +656,12 @@
 - r
 - r
 - y
-Now, we can count the occurrences of the letter 'r':
-- The first 'r' appears in the third position.
-- The second 'r' appears in the eighth position.
-- The third 'r' appears in the ninth position.
-Counting these, we find that there are a total of **3** 'r's in the word "strawberry."</t>
+Now, let's count the occurrences of the letter 'r':
+1. The first 'r' appears in the third position.
+2. The second 'r' appears in the eighth position.
+3. The third 'r' appears in the ninth position.
+Counting these, we find that there are a total of 3 'r's in the word "strawberry."
+Therefore, the answer is **3**.</t>
         </is>
       </c>
       <c r="D6" t="n">
@@ -676,7 +669,7 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>The model correctly identifies and counts the occurrences of 'r' in "strawberry," matching the expected output.</t>
+          <t>The model's answer correctly identifies and counts the occurrences of the letter 'r' in the word "strawberry," matching the expected output.</t>
         </is>
       </c>
     </row>
@@ -726,7 +719,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>the pattern is adding then minus 1. Thus, 3+4=7, 7-1 = 6. Final answer</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -743,11 +736,11 @@
         </is>
       </c>
       <c r="D8" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>The model correctly identifies the answer as 7 in standard arithmetic.</t>
+          <t>The model did not identify the pattern of adding then subtracting 1.</t>
         </is>
       </c>
     </row>
@@ -766,14 +759,14 @@
         <is>
           <t xml:space="preserve">1. She reached into the basket and picked the ripest fruit, an apple.  
 2. After a long day, he decided to treat himself to a healthy snack, an apple.  
-3. The teacher used a fruit to illustrate her lesson, choosing an apple.  
-4. In the garden, the tree was heavy with its sweetest harvest, an apple.  
-5. For dessert, they served a warm pie filled with slices of tart apple.  
-6. He always carried a piece of fruit in his bag, usually an apple.  
-7. The children giggled as they bobbed for the floating fruit, trying to catch an apple.  
-8. She smiled as she took a bite of her favorite fruit, a crisp apple.  
-9. The recipe called for a touch of sweetness, so she added an apple.  
-10. At the end of the picnic, they shared a simple treat, a juicy apple.  </t>
+3. The teacher used a simple illustration to explain the concept, featuring an apple.  
+4. In the garden, the tree was heavy with its seasonal bounty, including one shiny apple.  
+5. For dessert, they served a warm pie filled with sweet slices of apple.  
+6. As the sun set, the children enjoyed a picnic under the tree, sharing an apple.  
+7. He remembered the taste of his grandmother's famous dessert, which always included an apple.  
+8. The logo of the tech company is instantly recognizable, shaped like an apple.  
+9. She took a moment to appreciate the beauty of nature, focusing on a single, glistening apple.  
+10. At the market, he found the perfect ingredient for his recipe, a crisp apple.  </t>
         </is>
       </c>
       <c r="D9" t="n">
@@ -781,7 +774,7 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>The model's answer correctly provides 10 sentences ending with 'apple'.</t>
+          <t>All sentences correctly end with 'apple' as expected.</t>
         </is>
       </c>
     </row>
@@ -798,16 +791,16 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t xml:space="preserve">1. The first step in solving the puzzle is to gather all the clues, which leads us to the number 1.  
-2. After analyzing the data, we found that the most common response was the number 2.  
-3. In a game of chance, rolling a three is often considered a lucky outcome, so we celebrate the number 3.  
-4. The team scored four goals in the match, securing their victory with the number 4.  
-5. When counting the stars in the sky, I lost track after reaching the number 5.  
-6. The recipe calls for six ingredients, each contributing to the final dish, making it a total of 6.  
-7. During the experiment, we recorded seven different reactions, leading us to the conclusion of 7.  
-8. The marathon was completed by eight runners, each crossing the finish line with pride, resulting in the number 8.  
-9. In the final round of the quiz, the contestants answered nine questions correctly, showcasing their knowledge of the number 9.  
-10. The treasure hunt ended with a surprise, revealing ten hidden gems, which brings us to the number 10.  </t>
+          <t xml:space="preserve">1. The first step in solving the puzzle is to identify the clues that lead to the answer, which is 1.  
+2. In a race, the athlete who finishes ahead of everyone else takes home the gold medal, which is awarded to the winner, number 2.  
+3. When organizing a party, it's essential to have a guest list, and the first person on that list is number 3.  
+4. The four seasons of the year each bring their own unique beauty, but my favorite is the vibrant colors of autumn, which is represented by number 4.  
+5. In a standard deck of cards, the fifth card drawn can often change the outcome of the game, making it crucial to remember number 5.  
+6. The six continents of the world each have their own distinct cultures and landscapes, but I dream of visiting number 6.  
+7. When counting the days until the big event, I realized there were only seven left, which made me both excited and anxious for number 7.  
+8. The eight planets in our solar system each have their own unique characteristics, but I find the rings of Saturn particularly fascinating, which is number 8.  
+9. In a typical week, there are nine different opportunities to try something new, making every day an adventure for number 9.  
+10. Finally, the tenth chapter of the book reveals the most surprising twist in the story, leaving readers eager for more, which is number 10.  </t>
         </is>
       </c>
       <c r="D10" t="n">
@@ -815,7 +808,7 @@
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>The model's answer correctly provides 10 sentences ending with numbers 1 to 10.</t>
+          <t>The model provided 10 sentences ending with numbers 1 to 10, matching the expected output.</t>
         </is>
       </c>
     </row>
@@ -858,9 +851,9 @@
 height = 400
 display = pygame.display.set_mode((width, height))
 pygame.display.set_caption('Snake Game')
-# Set game clock
+# Set clock
 clock = pygame.time.Clock()
-# Set snake parameters
+# Set snake block size and speed
 snake_block = 10
 snake_speed = 15
 # Define font styles
@@ -869,6 +862,9 @@
 def our_snake(snake_block, snake_list):
     for x in snake_list:
         pygame.draw.rect(display, black, [x[0], x[1], snake_block, snake_block])
+def your_score(score):
+    value = score_font.render("Score: " + str(score), True, black)
+    display.blit(value, [0, 0])
 def message(msg, color):
     mesg = font_style.render(msg, True, color)
     display.blit(mesg, [width / 6, height / 3])
@@ -887,6 +883,7 @@
         while game_close == True:
             display.fill(blue)
             message("You Lost! Press C-Play Again or Q-Quit", red)
+            your_score(Length_of_snake - 1)
             pygame.display.update()
             for event in pygame.event.get():
                 if event.type == pygame.KEYDOWN:
@@ -927,6 +924,7 @@
             if x == snake_Head:
                 game_close = True
         our_snake(snake_block, snake_List)
+        your_score(Length_of_snake - 1)
         pygame.display.update()
         if x1 == foodx and y1 == foody:
             foodx = round(random.randrange(0, width - snake_block) / 10.0) * 10.0
@@ -939,7 +937,7 @@
 gameLoop()
 ```
 ### Step 3: Run the Game
-Save the above code in a file named `snake_game.py`. You can run the game by executing the following command in your terminal:
+Save the above code in a file named `snake_game.py` and run it using Python:
 ```bash
 python snake_game.py
 ```
@@ -947,16 +945,20 @@
 - Use the arrow keys to control the direction of the snake.
 - Press 'C' to play again after losing.
 - Press 'Q' to quit the game.
-### Conclusion
-This code provides a simple yet functional Snake game. You can enhance it further by adding features like scoring, levels, or sound effects. Enjoy coding and playing your Snake game!</t>
+### Explanation of the Code
+1. **Initialization**: The game initializes Pygame and sets up the display dimensions and colors.
+2. **Game Loop**: The main game loop handles events, updates the snake's position, checks for collisions, and updates the display.
+3. **Snake and Food**: The snake grows when it eats food, and the game ends if the snake collides with itself or the boundaries.
+4. **Score Display**: The current score is displayed on the screen.
+This code provides a basic implementation of the Snake game. You can enhance it further by adding features like levels, sound effects, or a more sophisticated scoring system. Enjoy coding!</t>
         </is>
       </c>
       <c r="D11" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>The model's answer is correct but includes extra information and uses different variable names and dimensions.</t>
+          <t>The model's answer is correct but includes extra information and a more detailed implementation than the expected output.</t>
         </is>
       </c>
     </row>
@@ -989,29 +991,23 @@
       <c r="C12" t="inlineStr">
         <is>
           <t>To solve this problem, we need to ensure that at no point are the cabbage and lion left alone together, nor are the lion and goat left alone together. Here’s a step-by-step plan to get all three across the river safely:
-1. **Take the lion across the river first.** 
-   - Now the cabbage and goat are on the original side, and the lion is on the other side.
-2. **Go back alone to the original side.**
-   - The cabbage and goat are still together, which is safe.
-3. **Take the goat across the river.**
-   - Now the lion and goat are on the other side, which is not allowed. So, we need to fix this.
-4. **Bring the lion back with you to the original side.**
-   - Now the lion is back with the cabbage, and the goat is alone on the other side.
-5. **Take the cabbage across the river.**
-   - Now the cabbage is on the other side, and the lion is back on the original side.
-6. **Go back alone to the original side.**
-   - The lion is alone, which is safe.
-7. **Finally, take the lion across the river.**
-   - Now all three (cabbage, goat, and lion) are safely on the other side.
-To summarize the steps:
-1. Take the lion across.
-2. Return alone.
-3. Take the goat across.
-4. Bring the lion back.
-5. Take the cabbage across.
-6. Return alone.
-7. Take the lion across.
-This way, at no point are the cabbage and lion or the lion and goat left alone together.</t>
+1. **Take the Lion Across First**: Start by taking the lion across the river. This leaves the goat and cabbage together on the original side, which is safe.
+2. **Return Alone**: Go back to the original side alone, leaving the lion on the other side.
+3. **Take the Goat Across**: Now, take the goat across the river.
+4. **Bring the Lion Back**: Leave the goat on the other side and take the lion back with you to the original side.
+5. **Take the Cabbage Across**: Leave the lion on the original side and take the cabbage across the river.
+6. **Return Alone**: Leave the cabbage with the goat on the other side and return alone to the original side.
+7. **Take the Lion Across Again**: Finally, take the lion across the river one last time.
+Now, all three—the cabbage, goat, and lion—are safely on the other side of the river without violating any of the conditions. 
+To summarize the crossings:
+- 1st trip: Lion across
+- 2nd trip: Return alone
+- 3rd trip: Goat across
+- 4th trip: Lion back
+- 5th trip: Cabbage across
+- 6th trip: Return alone
+- 7th trip: Lion across
+This sequence ensures that at no point are the cabbage and lion or the lion and goat left alone together.</t>
         </is>
       </c>
       <c r="D12" t="n">
@@ -1019,7 +1015,7 @@
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>The model's answer correctly follows the steps to ensure the lion is never left alone with the goat or the cabbage, matching the expected output.</t>
+          <t>The model's answer correctly follows the same steps as the expected output to ensure the lion is never left alone with the goat or cabbage.</t>
         </is>
       </c>
     </row>
@@ -1037,37 +1033,38 @@
       <c r="C13" t="inlineStr">
         <is>
           <t>To calculate the Return on Investment (ROI) for Vegan Steaks, we need to follow these steps:
-1. **Determine the Net Operating Profit**: 
-   The operating profit is given as $950,000. This is the net operating profit we will use in our ROI calculation.
+1. **Determine the Net Profit**: 
+   - The operating profit is given as $950,000. Since we are not provided with any interest or tax expenses, we will assume that the operating profit is equivalent to the net profit for this calculation.
 2. **Calculate the Average Investment**: 
-   The average investment can be calculated using the formula:
-   \[
-   \text{Average Investment} = \text{Cost of Assets} - \text{Accumulated Depreciation} + \text{Depreciation Expense}
-   \]
-   - Cost of Assets = $20,000,000
-   - Accumulated Depreciation = $5,000,000
-   - Depreciation Expense = $1,000,000
-   First, we calculate the net book value of the assets at the beginning of the year:
-   \[
-   \text{Net Book Value} = \text{Cost of Assets} - \text{Accumulated Depreciation} = 20,000,000 - 5,000,000 = 15,000,000
-   \]
-   Since the company did not buy any new assets during the year, the average investment remains the same as the net book value at the beginning of the year:
-   \[
-   \text{Average Investment} = 15,000,000
-   \]
+   - The average investment can be calculated using the formula:
+     \[
+     \text{Average Investment} = \text{Beginning Assets} - \text{Accumulated Depreciation} + \text{Depreciation Expense}
+     \]
+   - The beginning assets used in production are $20,000,000, and the accumulated depreciation at the beginning of the year is $5,000,000. The depreciation expense for the year is $1,000,000.
+   - Therefore, the net book value of the assets at the beginning of the year is:
+     \[
+     \text{Net Book Value} = \text{Beginning Assets} - \text{Accumulated Depreciation} = 20,000,000 - 5,000,000 = 15,000,000
+     \]
+   - Since no new assets were purchased during the year, the average investment remains the same as the net book value at the beginning of the year:
+     \[
+     \text{Average Investment} = 15,000,000
+     \]
 3. **Calculate ROI**: 
-   The ROI can be calculated using the formula:
-   \[
-   \text{ROI} = \left( \frac{\text{Net Operating Profit}}{\text{Average Investment}} \right) \times 100
-   \]
-   Substituting the values we have:
-   \[
-   \text{ROI} = \left( \frac{950,000}{15,000,000} \right) \times 100
-   \]
-   Now, calculate the ROI:
-   \[
-   \text{ROI} = \left( 0.0633333 \right) \times 100 \approx 6.33\%
-   \]
+   - The ROI can be calculated using the formula:
+     \[
+     \text{ROI} = \frac{\text{Net Profit}}{\text{Average Investment}} \times 100
+     \]
+   - Substituting the values we have:
+     \[
+     \text{ROI} = \frac{950,000}{15,000,000} \times 100
+     \]
+   - Performing the calculation:
+     \[
+     \text{ROI} = \frac{950,000}{15,000,000} = 0.0633333
+     \]
+     \[
+     \text{ROI} \approx 0.0633 \times 100 = 6.33\%
+     \]
 Thus, the ROI for Vegan Steaks for the year is approximately **6.33%**.</t>
         </is>
       </c>
@@ -1076,7 +1073,7 @@
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>The model's final ROI calculation is incorrect compared to the expected output of 6.55%.</t>
+          <t>The final ROI calculation is incorrect compared to the expected output.</t>
         </is>
       </c>
     </row>
@@ -1099,19 +1096,21 @@
 Now, let's analyze the situation after the guy kills one killer:
 - Before the killing: 2 killers in the room.
 - After the killing: 1 killer remains (since 1 killer was killed).
-However, we must also consider the guy who entered the room. He is not a killer by definition in this scenario, but he has committed a murder by killing one of the killers.
+However, we must also consider the guy who entered the room. He has now committed a murder, which means he has become a killer himself.
 So, after the incident:
-- 1 killer remains in the room.
-- The guy who entered the room is not counted as a killer in the original context.
-Thus, the total number of killers left in the room is **1**.</t>
+- 1 killer remains (the one who was not killed).
+- 1 new killer has been created (the guy who killed the first killer).
+Therefore, the total number of killers left in the room is:
+1 (remaining killer) + 1 (new killer) = 2 killers.
+So, there are 2 killers left in the room.</t>
         </is>
       </c>
       <c r="D14" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>The model's final answer is incorrect compared to the expected output.</t>
+          <t>The model's answer correctly explains the scenario and matches the expected output.</t>
         </is>
       </c>
     </row>
@@ -1131,39 +1130,41 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>To convert the provided bookstore inventory into JSON format, we need to structure the data as an array of objects, where each object represents a book with its title, author, and quantity. Here’s how it can be done step by step:
-1. Identify the key-value pairs for each book.
-2. Use proper JSON syntax, which includes using double quotes for keys and string values.
-3. Ensure that the entire structure is enclosed in square brackets to denote an array.
-Here’s the JSON representation of the bookstore inventory:
+          <t>To convert the provided bookstore inventory into JSON format, we need to structure the data as an array of objects, where each object represents a book with its title, author, and quantity. Here’s how it can be represented in JSON:
 ```json
-[
+{
+  "inventory": [
     {
-        "Title": "To Kill a Mockingbird",
-        "Author": "Harper Lee",
-        "Quantity": 30
+      "title": "To Kill a Mockingbird",
+      "author": "Harper Lee",
+      "quantity": 30
     },
     {
-        "Title": "1984",
-        "Author": "George Orwell",
-        "Quantity": 15
+      "title": "1984",
+      "author": "George Orwell",
+      "quantity": 15
     },
     {
-        "Title": "The Great Gatsby",
-        "Author": "F. Scott Fitzgerald",
-        "Quantity": 20
+      "title": "The Great Gatsby",
+      "author": "F. Scott Fitzgerald",
+      "quantity": 20
     }
-]
+  ]
+}
 ```
-This JSON format accurately represents the bookstore inventory with each book as an object in an array.</t>
+### Explanation:
+1. **Root Object**: The entire inventory is wrapped in a root object with a key called "inventory".
+2. **Array of Objects**: The value of "inventory" is an array (denoted by square brackets `[]`), containing multiple objects (denoted by curly braces `{}`).
+3. **Book Objects**: Each book is represented as an object with three key-value pairs: "title", "author", and "quantity". The keys are strings, and the values are either strings (for title and author) or numbers (for quantity). 
+This structure allows for easy access and manipulation of the bookstore inventory data.</t>
         </is>
       </c>
       <c r="D15" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>The model's answer correctly converts the bookstore inventory into JSON format but does not match the expected output structure.</t>
+          <t>The model's answer uses different key names and structure compared to the expected output.</t>
         </is>
       </c>
     </row>
@@ -1195,11 +1196,11 @@
           <t>To determine the maximum annual vacation accrual for full-time employees with more than 10 years of credited service, we can refer to the provided information.
 1. **Identify the category for employees with more than 10 years of credited service**:
    - The relevant section states: "Years of Credited Services &gt; 10 Years".
-2. **Find the maximum annual vacation accrual for this category**:
+2. **Look at the maximum annual vacation accrual for this category**:
    - According to the data, for full-time employees with more than 10 years of credited service, the maximum annual vacation accrual is **200 hours (25 days)**.
 3. **Check the maximum vacation accrual cap**:
    - The maximum vacation accrual cap for this category is **300 hours**.
-Thus, the maximum annual vacation accrual for full-time employees with more than 10 years of credited service is **200 hours (25 days)**.</t>
+Thus, for full-time employees with more than 10 years of credited service, the maximum annual vacation accrual is **200 hours (25 days)**.</t>
         </is>
       </c>
       <c r="D16" t="n">
@@ -1207,7 +1208,7 @@
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>The model's answer matches the expected output exactly.</t>
+          <t>The model's answer correctly identifies the maximum annual vacation accrual as 200 hours (25 days).</t>
         </is>
       </c>
     </row>
@@ -1227,14 +1228,12 @@
           <t>To analyze the situation regarding the use of vacation that was not accrued and the implications of leaving the company, let's break down the information provided step by step:
 1. **Understanding Accrued Vacation**: Accrued vacation refers to the vacation time that an employee has earned based on their time worked and the company's vacation policy. If you have not accrued vacation, it means you have taken more vacation time than you have earned.
 2. **Company Policy on Vacation Upon Leaving**: According to the Redhorse Paid Time Off Program FAQs, when an employee leaves the company, they will be paid for any unused and accrued vacation. This means that if you have vacation time that you have earned but not used, you will receive payment for that time.
-3. **Negative Vacation Balance**: If you have used vacation time that you did not accrue (resulting in a negative vacation balance), the policy states that upon termination of employment, the company has the right to withhold any amounts owed from your final paycheck. This means that if you took more vacation than you earned, the company can deduct that amount from what you would normally receive in your last paycheck.
-4. **Obligation to Repay**: The policy also indicates that if there are any additional amounts owed (in this case, the negative balance from unearned vacation), you will be required to repay that amount to Redhorse within 30 days of your last day of work.
-5. **California Employees**: The policy specifies that for California employees, the same rules apply regarding the repayment of negative vacation balances. However, California has specific labor laws that may provide additional protections for employees, so it’s important to be aware of those.
-### Conclusion:
-If you used vacation that was not accrued and then leave the company, you will likely face the following consequences:
-- Your final paycheck may be reduced by the amount of vacation time you took that you did not earn (negative balance).
-- You may be required to repay any additional amounts owed to the company within 30 days of your last day of work.
-It is advisable to review your specific situation with HR or a legal professional to understand your rights and obligations fully, especially if you are in California or if there are any other relevant state laws that may apply.</t>
+3. **Negative Vacation Balance**: The policy states that if an employee has a negative vacation balance (meaning they have taken more vacation than they have accrued), the company has the right to withhold amounts owed from the final paycheck. This applies to all non-California employees.
+4. **Implications of Using Non-Accrued Vacation**: If you used vacation that was not accrued (i.e., you took more vacation than you had earned), and then you leave the company, the following will happen:
+   - If you have a negative vacation balance, the company will withhold the amount owed for the vacation you took but did not earn from your final paycheck.
+   - If you owe more than what your final paycheck covers, you will be required to pay the remaining balance to Redhorse within 30 days of your last day of work.
+5. **California Employees**: The policy also specifies that for California employees, the same rules apply regarding negative vacation balances, and any amounts owed will be due within 30 days of the last day worked.
+**Conclusion**: If you used vacation that was not accrued and then leave the company, you will likely have a negative vacation balance. The company will withhold the amount owed from your final paycheck, and if that amount exceeds your final paycheck, you will need to pay the remaining balance to the company within 30 days. It is important to be aware of this policy to avoid any unexpected financial obligations upon leaving the company.</t>
         </is>
       </c>
       <c r="D17" t="n">

</xml_diff>